<commit_message>
feat: Refactor role and user edit pages to use Suspense and improve loading states
- Updated EditRolePage and EditUserPage to utilize Suspense for loading forms.
- Introduced FormSkeleton component for better user experience during data fetching.
- Refactored RoleForm and UserForm components to streamline form rendering.
- Enhanced error handling for unauthorized and not found responses in role and user fetching.
- Improved pagination and search functionality in RolePage and UserPage.
- Added TreeViewSkeleton and PvFormSkeleton components for loading states in respective views.
- Implemented new action for PDF generation in list-payment feature.
- Updated SearchBox debounce timing for improved performance.
- Enhanced UI components such as Checkbox and Table for better accessibility and usability.
</commit_message>
<xml_diff>
--- a/public/template/upload_rv.xlsx
+++ b/public/template/upload_rv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ky0sh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prima\nextjs\klik\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77CCAF0A-30AE-4AD7-9D6A-5BE1487C49FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA886AD-287D-4A37-8530-B9BC5659EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34BBA9E7-0AA5-4D10-AF00-91371A3B3BC2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Tgl Event</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>929489</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>KLIKLELANG-Eddy susiyanto</t>
   </si>
 </sst>
 </file>
@@ -72,7 +78,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -162,13 +168,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B76B30-49DC-4880-A317-EE82F9873759}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,12 +501,13 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,16 +518,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45964</v>
       </c>
@@ -530,13 +540,16 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>8450000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Refactor role and user edit pages to use Suspense and improve loading states (#10)
- Updated EditRolePage and EditUserPage to utilize Suspense for loading forms.
- Introduced FormSkeleton component for better user experience during data fetching.
- Refactored RoleForm and UserForm components to streamline form rendering.
- Enhanced error handling for unauthorized and not found responses in role and user fetching.
- Improved pagination and search functionality in RolePage and UserPage.
- Added TreeViewSkeleton and PvFormSkeleton components for loading states in respective views.
- Implemented new action for PDF generation in list-payment feature.
- Updated SearchBox debounce timing for improved performance.
- Enhanced UI components such as Checkbox and Table for better accessibility and usability.
</commit_message>
<xml_diff>
--- a/public/template/upload_rv.xlsx
+++ b/public/template/upload_rv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ky0sh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prima\nextjs\klik\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77CCAF0A-30AE-4AD7-9D6A-5BE1487C49FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA886AD-287D-4A37-8530-B9BC5659EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34BBA9E7-0AA5-4D10-AF00-91371A3B3BC2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Tgl Event</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>929489</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>KLIKLELANG-Eddy susiyanto</t>
   </si>
 </sst>
 </file>
@@ -72,7 +78,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -162,13 +168,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B76B30-49DC-4880-A317-EE82F9873759}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,12 +501,13 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,16 +518,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45964</v>
       </c>
@@ -530,13 +540,16 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>8450000</v>
       </c>
     </row>

</xml_diff>